<commit_message>
Updated comments and Jπ
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B33BB8-2BA1-454B-8213-6A4DB29A8916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7913C011-57FF-4C89-ADF3-BD664FB0A497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1164,54 +1164,56 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>20</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <f t="shared" ref="C13:G14" si="14">C31</f>
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="4">
         <f t="shared" si="14"/>
         <v>37</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="4">
         <v>2</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="4">
         <v>33</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="5">
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">

</xml_diff>

<commit_message>
Update Mg35 ENSDF files with revised data and remove outdated entries
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278124EB-DB40-4BB6-96D4-F3E3C6A3E402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C1369-C102-49E8-8D93-1432931AF696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -752,7 +752,9 @@
         <f t="shared" ref="M3:M14" si="4">L3</f>
         <v>8</v>
       </c>
-      <c r="N3" s="5"/>
+      <c r="N3" s="5">
+        <v>20250509</v>
+      </c>
       <c r="O3" s="5">
         <f>I3</f>
         <v>0</v>
@@ -811,7 +813,9 @@
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="N4" s="5"/>
+      <c r="N4" s="5">
+        <v>20250516</v>
+      </c>
       <c r="O4" s="5">
         <v>1</v>
       </c>
@@ -870,7 +874,7 @@
         <v>57</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O4:O10" si="8">I5</f>
+        <f t="shared" ref="O5:O10" si="8">I5</f>
         <v>3</v>
       </c>
       <c r="P5" s="8">

</xml_diff>

<commit_message>
Update ENSDF files for Mg35 and Ca35 with revised data and improved documentation
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C1369-C102-49E8-8D93-1432931AF696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AA555C-257A-428A-97D2-F01CD7523C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -825,59 +825,62 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="2">
         <v>12</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <f t="shared" ref="C5:G5" si="7">C23</f>
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <f t="shared" si="7"/>
         <v>243</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <f t="shared" si="0"/>
         <v>243</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="9">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>3</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="5">
         <v>57</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="9">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="O5" s="4">
+      <c r="N5" s="5">
+        <v>20250522</v>
+      </c>
+      <c r="O5" s="5">
         <f t="shared" ref="O5:O10" si="8">I5</f>
         <v>3</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="9">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Add new datasets and updates for 35Al
- Introduced a new dataset for the Coulomb dissociation of 35Al using a Pb target, compiled from 2017Ch36.
- Added a dataset for the beta-neutron decay of 36Mg, compiled from 2023Lu07.
- Updated the one-proton knockout reaction dataset for 9Be(36Si,35Al) based on 2014St18.
- Included a new dataset for the Coulomb excitation of 35Al from 1999Ib01.
- Added adopted levels and gamma data for 35Al, consolidating previous evaluations and measurements.
- Updated the dataset for the Coulomb dissociation of 35Al on Pb target, reflecting new findings and configurations.
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AA555C-257A-428A-97D2-F01CD7523C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02098585-CDDE-4E07-9355-7DED3B16CD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -596,13 +596,14 @@
     <col min="6" max="6" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -817,11 +818,11 @@
         <v>20250516</v>
       </c>
       <c r="O4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" s="9">
         <f t="shared" ref="P4:P14" si="6">O4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -886,59 +887,60 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="2">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <f t="shared" ref="C6:G6" si="9">C24</f>
         <v>8</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <f t="shared" si="9"/>
         <v>27</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <f t="shared" si="9"/>
         <v>258</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="9">
         <f t="shared" si="0"/>
         <v>258</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="9">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>4</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
         <v>48</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="9">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="O6" s="4">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="9">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Update change log and refine theoretical NSRs for Ar35, P35, K35, Mg35, and Na35 datasets; add new beta decay data for Al35.
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02098585-CDDE-4E07-9355-7DED3B16CD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F569308-BAC3-42D1-9348-E1DF58D3D5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -875,7 +875,7 @@
         <v>57</v>
       </c>
       <c r="N5" s="5">
-        <v>20250522</v>
+        <v>20250528</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" ref="O5:O10" si="8">I5</f>

</xml_diff>

<commit_message>
Revised Al and Mg
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F569308-BAC3-42D1-9348-E1DF58D3D5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735356FE-A681-4BFB-94BF-59F68C8D08E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -187,7 +187,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,12 +206,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCECFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -225,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,9 +249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +575,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -935,72 +926,73 @@
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="N6" s="5">
+        <v>20250530</v>
+      </c>
       <c r="O6" s="5">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P6" s="9">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="2">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <f t="shared" ref="C7:G7" si="10">C25</f>
         <v>21</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <f t="shared" si="10"/>
         <v>53</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <f t="shared" si="10"/>
         <v>386</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <f t="shared" si="0"/>
         <v>386</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="9">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>3</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="5">
         <v>65</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="9">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="O7" s="4">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="P7" s="8">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5">
+        <v>5</v>
+      </c>
+      <c r="P7" s="9">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: Update Si35 ENSDF file and Copilot instructions
Updates include:
- Corrected G-record spacing in Si35_35al_beta_decay_38.1_ms.ens.
- Added E(n0){-c.m.} comments to Si35_35al_beta_decay_38.1_ms.ens.
- Corrected 35Si to {+35}Si in Si35_35al_beta_decay_38.1_ms.ens.
- Deleted 'D' flags from column 77 in Beta (B) records in Si35_35al_beta_decay_38.1_ms.ens.
- Updated .vscode/copilot-instructions.md with ENSDF 'G' record formatting rules.
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735356FE-A681-4BFB-94BF-59F68C8D08E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50494C97-B721-48A3-83DA-C90877148DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -927,14 +927,14 @@
         <v>48</v>
       </c>
       <c r="N6" s="5">
-        <v>20250530</v>
+        <v>20250603</v>
       </c>
       <c r="O6" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P6" s="9">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -986,7 +986,9 @@
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="N7" s="5">
+        <v>20250610</v>
+      </c>
       <c r="O7" s="5">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
feat: Add comprehensive ENSDF formatting guide and Fix Format command
- Add complete ENSDF special character reference with Greek letters and math symbols
- Implement "Fix Format" quick command for automated ENSDF notation conversion
- Streamline copilot-instructions.md organization and remove redundancies
- Convert reaction notation to proper ENSDF format in P35_160gd_37cl_xg.ens
- Fix grammar and apply ENSDF formatting to S35_208pb_36s_xg.ens shell model configs
- Document Si35_208pb_36s_xg.ens containing 208PB(36S,XG) reaction data
- Update change log with proper reverse chronological order (2025-06-16 first)
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50494C97-B721-48A3-83DA-C90877148DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BC2372-1C1B-4AAA-9E34-9DF9A5F65ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -202,7 +202,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -251,6 +251,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,6 +268,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFCCECFF"/>
       <color rgb="FFFF5353"/>
@@ -575,7 +585,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -590,7 +600,7 @@
     <col min="9" max="9" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="1" bestFit="1" customWidth="1"/>
@@ -990,11 +1000,11 @@
         <v>20250610</v>
       </c>
       <c r="O7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P7" s="9">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1050,11 +1060,11 @@
         <v>20250324</v>
       </c>
       <c r="O8" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P8" s="9">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1064,62 +1074,63 @@
       <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="11">
         <f t="shared" ref="C9:G9" si="12">C27</f>
         <v>141</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="11">
         <f t="shared" si="12"/>
         <v>136</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="11">
         <f t="shared" si="12"/>
         <v>393</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="11">
         <f t="shared" si="12"/>
         <v>310</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="11">
         <f t="shared" si="12"/>
         <v>1043</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="12">
         <f t="shared" si="0"/>
         <v>1043</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="11">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="11">
         <v>4</v>
       </c>
-      <c r="L9" s="4">
-        <v>306</v>
-      </c>
-      <c r="M9" s="8">
+      <c r="L9" s="11">
+        <v>309</v>
+      </c>
+      <c r="M9" s="12">
         <f t="shared" si="4"/>
-        <v>306</v>
-      </c>
-      <c r="O9" s="4">
+        <v>309</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="12">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="13">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
@@ -1158,11 +1169,11 @@
         <v>10</v>
       </c>
       <c r="L10" s="4">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" si="4"/>
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="8"/>
@@ -1276,11 +1287,11 @@
         <v>0</v>
       </c>
       <c r="L12" s="5">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M12" s="9">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N12" s="5">
         <v>20250506</v>
@@ -1409,6 +1420,12 @@
       <c r="P14" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L15" s="4">
+        <f>SUM(L3:L14)</f>
+        <v>1475</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
A35 evaluation: Citation tense fixes, symbol encoding corrections, and file reorganization
- Fixed academic citation tense throughout A35 files (states → stated)
- Corrected ENSDF approximate value encoding (~ → |? for numeric values)
- Renamed S35_208pb_36s_xg.ens → S35_208pb_36s_35sg.ens for clarity
- Updated copilot instructions with citation guidelines and symbol encoding
- Applied scientific writing conventions across K35, P35, Ar35, and S35 datasets
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BC2372-1C1B-4AAA-9E34-9DF9A5F65ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDC2BE3-8A59-48C1-B6EC-8B921EAB8CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -585,7 +585,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -997,7 +997,7 @@
         <v>65</v>
       </c>
       <c r="N7" s="5">
-        <v>20250610</v>
+        <v>20250616</v>
       </c>
       <c r="O7" s="5">
         <v>6</v>

</xml_diff>

<commit_message>
Add weekly effort log for nuclear structure and decay data evaluation
- Documented progress from February to June 2025, detailing training received, datasets completed, and collaborations.
- Included responsibilities and duties related to ENSDF evaluation, XUNDL compilation, and data consistency checks.
- Highlighted technical development efforts and research outputs, including coauthored papers.
- Emphasized collaborations with FRIB Laboratory, USNDP, NSDD, and BEApR evaluators.
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDC2BE3-8A59-48C1-B6EC-8B921EAB8CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17196CE-2A0D-45F9-A0F3-9FEFEDAAD88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -585,7 +585,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add new ENSDF data for 35S and XUNDL-5 dataset for 34S(D,PG)
- Introduced a new ENSDF file for 35S, detailing experimental results from 2015MuZY, including inclusive cross sections, spectroscopic factors, and decay properties.
- Added an XUNDL-5 dataset for 34S(D,PG) compiled from 2024Co04, documenting the experimental setup and results from the John D. Fox Superconducting Linear Accelerator Laboratory.
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17196CE-2A0D-45F9-A0F3-9FEFEDAAD88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2879A060-18B5-40F2-83F0-CD782CF07C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E3F13E08-64ED-4767-9D40-D1E60D65A10A}"/>
   </bookViews>
@@ -585,7 +585,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1107,7 +1107,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L9" s="11">
         <v>309</v>
@@ -1118,12 +1118,11 @@
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11">
-        <f t="shared" si="8"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P9" s="12">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1227,11 +1226,11 @@
         <v>5</v>
       </c>
       <c r="L11" s="5">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="M11" s="9">
         <f t="shared" si="4"/>
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N11" s="5">
         <v>20250425</v>
@@ -1425,7 +1424,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L15" s="4">
         <f>SUM(L3:L14)</f>
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>